<commit_message>
Site updated at: 2017-09-13 07:19:09 UTC
</commit_message>
<xml_diff>
--- a/class/seminar_core_areas_learning/coin.xlsx
+++ b/class/seminar_core_areas_learning/coin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" activeTab="2" xr2:uid="{48EC1B71-28FA-411D-92FC-A059623DD727}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120" activeTab="1" xr2:uid="{48EC1B71-28FA-411D-92FC-A059623DD727}"/>
   </bookViews>
   <sheets>
     <sheet name="コイン" sheetId="2" r:id="rId1"/>
@@ -292,15 +292,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>コインの</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ja-JP"/>
-              <a:t>2</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>項分布</a:t>
+              <a:t>コインの確率</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -755,15 +747,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>コインの</a:t>
+              <a:t>コインの表が</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ja-JP"/>
-              <a:t>2</a:t>
+              <a:t>k</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>項分布（理想）</a:t>
+              <a:t>回出る確率</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -961,6 +953,11 @@
                   <a:rPr lang="ja-JP" altLang="en-US"/>
                   <a:t>表が出る回数</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>k</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1236,7 +1233,15 @@
             </a:r>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>項分布（理想）</a:t>
+              <a:t>以下が</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>k</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>回出る確率</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1427,6 +1432,11 @@
                   <a:rPr lang="ja-JP" altLang="en-US"/>
                   <a:t>以下が出る回数</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>k</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -7800,8 +7810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ECEDA0-9210-4340-ADC2-670D99A5F772}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7975,8 +7985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BB2295-9ACC-4F2D-B4DF-E7AC79F31253}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -8107,7 +8117,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>